<commit_message>
update images + add image for february 2022
</commit_message>
<xml_diff>
--- a/statistics_files/2022/2022.z.graph.xlsx
+++ b/statistics_files/2022/2022.z.graph.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20382"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20383"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Linked in NEXT\Statistics\2021\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\Documents\GitHub\next_statistics\statistics_files\2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52473C4C-5E08-434A-9DBA-730E9BC19855}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8934160-8FAA-452B-A64A-17450D68C99B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11685" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1046,6 +1046,9 @@
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>80460</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>74752</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2130,7 +2133,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2193,6 +2198,9 @@
       <c r="E3">
         <v>62889</v>
       </c>
+      <c r="F3">
+        <v>74752</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">

</xml_diff>

<commit_message>
Update image for march
</commit_message>
<xml_diff>
--- a/statistics_files/2022/2022.z.graph.xlsx
+++ b/statistics_files/2022/2022.z.graph.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20383"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20384"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\Documents\GitHub\next_statistics\statistics_files\2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8934160-8FAA-452B-A64A-17450D68C99B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90DB5583-C725-4200-AA60-F2B5F3AD3E9A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11685" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1049,6 +1049,9 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>74752</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>90284</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2133,9 +2136,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2218,6 +2219,9 @@
       <c r="E4">
         <v>82434</v>
       </c>
+      <c r="F4">
+        <v>90284</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">

</xml_diff>

<commit_message>
Update graph and graph making excel file
</commit_message>
<xml_diff>
--- a/statistics_files/2022/2022.z.graph.xlsx
+++ b/statistics_files/2022/2022.z.graph.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20384"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20386"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\Documents\GitHub\next_statistics\statistics_files\2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E1A99D6-6C12-4464-8F31-CAC6815EEA89}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A56C314A-560A-40D2-8FC8-4928A0BEF99D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11685" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1051,6 +1051,12 @@
                   <c:v>74752</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>90284</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>82578</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>90284</c:v>
                 </c:pt>
               </c:numCache>
@@ -2136,7 +2142,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2239,6 +2247,9 @@
       <c r="E5">
         <v>75969</v>
       </c>
+      <c r="F5">
+        <v>82578</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -2255,6 +2266,9 @@
       </c>
       <c r="E6">
         <v>74398</v>
+      </c>
+      <c r="F6">
+        <v>90284</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update graph for June
</commit_message>
<xml_diff>
--- a/statistics_files/2022/2022.z.graph.xlsx
+++ b/statistics_files/2022/2022.z.graph.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20386"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20387"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\Documents\GitHub\next_statistics\statistics_files\2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A56C314A-560A-40D2-8FC8-4928A0BEF99D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8332E6F8-9919-452B-8602-BE302143BDCC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11685" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1058,6 +1058,9 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>90284</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>115115</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2287,6 +2290,9 @@
       <c r="E7">
         <v>112681</v>
       </c>
+      <c r="F7">
+        <v>115115</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">

</xml_diff>

<commit_message>
Update image files for September 2022
</commit_message>
<xml_diff>
--- a/statistics_files/2022/2022.z.graph.xlsx
+++ b/statistics_files/2022/2022.z.graph.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20387"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20390"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\Documents\GitHub\next_statistics\statistics_files\2022\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\Documents\github\next_statistics\statistics_files\2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B40E7A7-4619-4EAB-AB8C-C6F14754BFCB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C92CE6E-54EF-4AD2-AB2D-E5B9AA1950F5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11685" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11690" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1064,6 +1064,12 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>102360</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>101787</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90267</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2148,16 +2154,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2177,7 +2183,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -2197,7 +2203,7 @@
         <v>80460</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2217,7 +2223,7 @@
         <v>74752</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -2237,7 +2243,7 @@
         <v>90284</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -2257,7 +2263,7 @@
         <v>82578</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -2277,7 +2283,7 @@
         <v>90284</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -2297,7 +2303,7 @@
         <v>115115</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -2317,7 +2323,7 @@
         <v>102360</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -2333,8 +2339,11 @@
       <c r="E9">
         <v>90273</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <v>101787</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -2350,8 +2359,11 @@
       <c r="E10">
         <v>84093</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F10">
+        <v>90267</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -2368,7 +2380,7 @@
         <v>85168</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -2385,7 +2397,7 @@
         <v>81583</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -2402,7 +2414,7 @@
         <v>75582</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>13</v>
       </c>
@@ -2412,7 +2424,7 @@
       <c r="E16" s="3"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -2420,7 +2432,7 @@
       <c r="E17" s="3"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -2428,7 +2440,7 @@
       <c r="E18" s="3"/>
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -2436,7 +2448,7 @@
       <c r="E19" s="3"/>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -2444,7 +2456,7 @@
       <c r="E20" s="3"/>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -2452,7 +2464,7 @@
       <c r="E21" s="3"/>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -2460,7 +2472,7 @@
       <c r="E22" s="3"/>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -2468,7 +2480,7 @@
       <c r="E23" s="3"/>
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -2476,7 +2488,7 @@
       <c r="E24" s="3"/>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -2484,7 +2496,7 @@
       <c r="E25" s="3"/>
       <c r="F25" s="1"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -2492,7 +2504,7 @@
       <c r="E26" s="3"/>
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -2500,7 +2512,7 @@
       <c r="E27" s="3"/>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -2508,7 +2520,7 @@
       <c r="E28" s="3"/>
       <c r="F28" s="1"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -2516,7 +2528,7 @@
       <c r="E29" s="3"/>
       <c r="F29" s="1"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>

</xml_diff>

<commit_message>
add files and update A
</commit_message>
<xml_diff>
--- a/statistics_files/2022/2022.z.graph.xlsx
+++ b/statistics_files/2022/2022.z.graph.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20391"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20392"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\Documents\GitHub\next_statistics\statistics_files\2022\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\Documents\github\next_statistics\statistics_files\2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49A9572F-2730-4A40-93C9-2E79FB595000}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A266BAA-CE9B-4559-A467-2D32D6738E43}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11685" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11690" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1073,6 +1073,9 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>87376</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>84228</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2158,15 +2161,15 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2186,7 +2189,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -2206,7 +2209,7 @@
         <v>80460</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2226,7 +2229,7 @@
         <v>74752</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -2246,7 +2249,7 @@
         <v>90284</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -2266,7 +2269,7 @@
         <v>82578</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -2286,7 +2289,7 @@
         <v>90284</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -2306,7 +2309,7 @@
         <v>115115</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -2326,7 +2329,7 @@
         <v>102360</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -2346,7 +2349,7 @@
         <v>101787</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -2366,7 +2369,7 @@
         <v>90267</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -2386,7 +2389,7 @@
         <v>87376</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -2402,8 +2405,11 @@
       <c r="E12">
         <v>81583</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F12">
+        <v>84228</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -2420,7 +2426,7 @@
         <v>75582</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>13</v>
       </c>
@@ -2430,7 +2436,7 @@
       <c r="E16" s="3"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -2438,7 +2444,7 @@
       <c r="E17" s="3"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -2446,7 +2452,7 @@
       <c r="E18" s="3"/>
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -2454,7 +2460,7 @@
       <c r="E19" s="3"/>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -2462,7 +2468,7 @@
       <c r="E20" s="3"/>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -2470,7 +2476,7 @@
       <c r="E21" s="3"/>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -2478,7 +2484,7 @@
       <c r="E22" s="3"/>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -2486,7 +2492,7 @@
       <c r="E23" s="3"/>
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -2494,7 +2500,7 @@
       <c r="E24" s="3"/>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -2502,7 +2508,7 @@
       <c r="E25" s="3"/>
       <c r="F25" s="1"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -2510,7 +2516,7 @@
       <c r="E26" s="3"/>
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -2518,7 +2524,7 @@
       <c r="E27" s="3"/>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -2526,7 +2532,7 @@
       <c r="E28" s="3"/>
       <c r="F28" s="1"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -2534,7 +2540,7 @@
       <c r="E29" s="3"/>
       <c r="F29" s="1"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>

</xml_diff>